<commit_message>
040125 EOD finished 4 integrations
</commit_message>
<xml_diff>
--- a/Daily Activity/2025/2025 Worksheet.xlsx
+++ b/Daily Activity/2025/2025 Worksheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t xml:space="preserve">DATE</t>
   </si>
@@ -92,6 +92,28 @@
   </si>
   <si>
     <t xml:space="preserve">YES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imported Promotion
+Order in UAT for 7 regions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manirathnam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tested centra. Bugs found(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inprogress</t>
   </si>
 </sst>
 </file>
@@ -107,6 +129,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -134,7 +157,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -192,7 +214,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -205,11 +227,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -293,32 +323,31 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="26.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="4.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="21.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="9.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="7.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="26.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="12.3"/>
   </cols>
   <sheetData>
@@ -401,14 +430,47 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <v>45659</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>45660</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>8098</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
070125 EOD Completed NTA AP Payment testing in centra
</commit_message>
<xml_diff>
--- a/Daily Activity/2025/2025 Worksheet.xlsx
+++ b/Daily Activity/2025/2025 Worksheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t xml:space="preserve">DATE</t>
   </si>
@@ -117,6 +117,10 @@
   </si>
   <si>
     <t xml:space="preserve">Prepard KT Documents for integrations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tested Purchase Management
+GR and AP Invoice Bugs found(2)</t>
   </si>
 </sst>
 </file>
@@ -242,8 +246,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -326,14 +330,15 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="34.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.56"/>
@@ -475,6 +480,9 @@
       <c r="H4" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="J4" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
@@ -483,7 +491,7 @@
       <c r="D5" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>31</v>
       </c>
       <c r="F5" s="0" t="s">
@@ -504,9 +512,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
         <v>45663</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>8098</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
17/01/25 EOD completed accounting user
</commit_message>
<xml_diff>
--- a/Daily Activity/2025/2025 Worksheet.xlsx
+++ b/Daily Activity/2025/2025 Worksheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Jan-01" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="55">
   <si>
     <t xml:space="preserve">DATE</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tested ACL CheckList for user PHAMCX7(185 SR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tested ACL CheckList for user TANGTX23</t>
   </si>
   <si>
     <t xml:space="preserve">MONTH</t>
@@ -198,7 +201,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -226,17 +229,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -393,7 +385,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -401,7 +393,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -492,11 +484,11 @@
   </sheetPr>
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.33"/>
@@ -820,23 +812,41 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="n">
+    <row r="15" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="n">
         <v>45671</v>
       </c>
-    </row>
-    <row r="16" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="n">
+      <c r="B15" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="13" t="n">
         <v>45672</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6" t="s">
+      <c r="B16" s="14"/>
+      <c r="C16" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="n">
         <v>45673</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>8098</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,27 +942,27 @@
   </sheetPr>
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="4.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="7.68"/>
@@ -1193,32 +1203,32 @@
   <dimension ref="F5:I19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F5" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F6" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G6" s="18" t="n">
         <f aca="false">COUNTIF('Jan-01'!B2:B32,"YES")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H6" s="19" t="n">
         <f aca="false">COUNTIF('Jan-01'!C2:C32,"YES")</f>
@@ -1231,7 +1241,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F7" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
@@ -1239,7 +1249,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F8" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
@@ -1247,7 +1257,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F9" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
@@ -1255,7 +1265,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F10" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -1263,7 +1273,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F11" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
@@ -1271,7 +1281,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F12" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
@@ -1279,7 +1289,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F13" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
@@ -1287,7 +1297,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F14" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
@@ -1295,7 +1305,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F15" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
@@ -1303,7 +1313,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F16" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
@@ -1311,7 +1321,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F17" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
@@ -1325,11 +1335,11 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F19" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G19" s="20" t="n">
         <f aca="false">SUM(G6:G17)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H19" s="20" t="n">
         <f aca="false">SUM(H6:H17)</f>

</xml_diff>

<commit_message>
180125 EOD checked RO Transformation
</commit_message>
<xml_diff>
--- a/Daily Activity/2025/2025 Worksheet.xlsx
+++ b/Daily Activity/2025/2025 Worksheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="55">
   <si>
     <t xml:space="preserve">DATE</t>
   </si>
@@ -484,11 +484,11 @@
   </sheetPr>
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.33"/>
@@ -853,6 +853,21 @@
       <c r="A18" s="7" t="n">
         <v>45674</v>
       </c>
+      <c r="D18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>8098</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="n">
@@ -946,7 +961,7 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.47"/>
@@ -955,7 +970,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.46"/>
@@ -1206,7 +1221,7 @@
       <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F5" s="16" t="s">

</xml_diff>